<commit_message>
permirsimi i emrit te rruges
</commit_message>
<xml_diff>
--- a/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-1084-29-Fahriu.xlsx
+++ b/4-Te-dhenat-per-kataster/regjistri/17-Regjistri-i-ndërrimeve-për-ndertesë-1084-29-Fahriu.xlsx
@@ -104,9 +104,6 @@
     <t>P+1</t>
   </si>
   <si>
-    <t>Rr. " Rexhep Bislimi "</t>
-  </si>
-  <si>
     <t>Fahri (Beqir) Salihu</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>O-72217092-01084-29-____-___</t>
+  </si>
+  <si>
+    <t>Rr. " Besim Rexhepi "</t>
   </si>
 </sst>
 </file>
@@ -473,48 +473,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -538,6 +496,48 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -931,7 +931,7 @@
   <dimension ref="A1:Q668"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,170 +954,170 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+      <c r="N4" s="22"/>
+      <c r="O4" s="22"/>
+      <c r="P4" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
+      <c r="A5" s="22"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
+      <c r="A6" s="22"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="A7" s="22"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="15"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="18"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="26"/>
     </row>
     <row r="10" spans="1:17" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1153,11 +1153,11 @@
       <c r="K10" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L10" s="19" t="s">
+      <c r="L10" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="19"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
       <c r="O10" s="10" t="s">
         <v>9</v>
       </c>
@@ -1166,19 +1166,19 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="30">
         <v>1</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="20" t="s">
+      <c r="D11" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="28" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -1187,60 +1187,60 @@
       <c r="G11" s="12">
         <v>138.66999999999999</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="28">
         <v>114.3</v>
       </c>
-      <c r="I11" s="20" t="s">
+      <c r="I11" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="J11" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="20">
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="28">
         <v>1011633893</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="32" t="s">
         <v>6</v>
       </c>
       <c r="Q11" s="6"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
       <c r="F12" s="11" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="11">
         <v>118.8</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="24"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="32"/>
       <c r="Q12" s="6"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
       <c r="F13" s="13" t="s">
         <v>23</v>
       </c>
@@ -1248,15 +1248,15 @@
         <f>SUM(G11:G12)</f>
         <v>257.46999999999997</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="21"/>
-      <c r="P13" s="25"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="33"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L14" s="1"/>
@@ -1282,46 +1282,46 @@
     <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+      <c r="A21" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="32" t="s">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32" t="s">
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="34"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="20"/>
     </row>
     <row r="22" spans="1:16" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="30"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="35"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="19"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="21"/>
     </row>
     <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1644,6 +1644,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O11:O13"/>
+    <mergeCell ref="P11:P13"/>
+    <mergeCell ref="L11:N13"/>
     <mergeCell ref="A21:D22"/>
     <mergeCell ref="E21:H22"/>
     <mergeCell ref="I21:P22"/>
@@ -1660,9 +1663,6 @@
     <mergeCell ref="I11:I13"/>
     <mergeCell ref="J11:J13"/>
     <mergeCell ref="K11:K13"/>
-    <mergeCell ref="O11:O13"/>
-    <mergeCell ref="P11:P13"/>
-    <mergeCell ref="L11:N13"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>